<commit_message>
adds petal weight data sets revises script for merging and analyzing petal traits.
</commit_message>
<xml_diff>
--- a/data/raw/plant/petal_weight.xlsx
+++ b/data/raw/plant/petal_weight.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\900008049\Documents\GitHub\CApoppy\data\raw\plant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gretchen/GitHub/CApoppy/data/raw/plant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D088814-4627-4E5F-B102-A962F792AF0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011C0418-522C-3345-88D6-48E2D7A720BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="760" windowWidth="33520" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38640" yWindow="500" windowWidth="33520" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Petal_2025_low" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -60,11 +73,17 @@
   <si>
     <t>water_mg</t>
   </si>
+  <si>
+    <t>water_percent</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -104,8 +123,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,17 +467,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -482,9 +501,12 @@
       <c r="H1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -509,13 +531,13 @@
         <f>D3-G3</f>
         <v>0.14157</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <f>H3/D3</f>
         <v>0.88942639944713198</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -540,13 +562,13 @@
         <f t="shared" ref="H4:H17" si="0">D4-G4</f>
         <v>9.8930000000000004E-2</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <f t="shared" ref="I4:I17" si="1">H4/D4</f>
         <v>0.89854677565849228</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -571,13 +593,13 @@
         <f t="shared" si="0"/>
         <v>0.18359</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <f t="shared" si="1"/>
         <v>0.89634801288936627</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
@@ -599,13 +621,13 @@
         <f t="shared" si="0"/>
         <v>0.15789999999999998</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <f t="shared" si="1"/>
         <v>0.89858866378329161</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
@@ -627,13 +649,13 @@
         <f t="shared" si="0"/>
         <v>0.16696</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <f t="shared" si="1"/>
         <v>0.89312078741842305</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
@@ -655,13 +677,13 @@
         <f t="shared" si="0"/>
         <v>0.14959</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <f t="shared" si="1"/>
         <v>0.89126549094375607</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
@@ -683,13 +705,13 @@
         <f t="shared" si="0"/>
         <v>0.10836</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <f t="shared" si="1"/>
         <v>0.88140556368960477</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
@@ -711,13 +733,13 @@
         <f t="shared" si="0"/>
         <v>0.13807</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="1">
         <f t="shared" si="1"/>
         <v>0.89498930446619562</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
@@ -739,13 +761,13 @@
         <f t="shared" si="0"/>
         <v>9.7549999999999998E-2</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <f t="shared" si="1"/>
         <v>0.89503624185705111</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B12" t="s">
@@ -767,13 +789,13 @@
         <f t="shared" si="0"/>
         <v>0.16535</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <f t="shared" si="1"/>
         <v>0.89986394557823124</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
@@ -795,13 +817,13 @@
         <f t="shared" si="0"/>
         <v>0.17779</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <f t="shared" si="1"/>
         <v>0.88673316708229422</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
@@ -823,13 +845,13 @@
         <f t="shared" si="0"/>
         <v>0.21931</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <f t="shared" si="1"/>
         <v>0.8932833693128589</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
@@ -851,13 +873,13 @@
         <f t="shared" si="0"/>
         <v>0.16967000000000002</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="1">
         <f t="shared" si="1"/>
         <v>0.89796242392167247</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B16" t="s">
@@ -879,13 +901,13 @@
         <f t="shared" si="0"/>
         <v>0.12121</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="1">
         <f t="shared" si="1"/>
         <v>0.8909879447221406</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="s">
@@ -907,13 +929,13 @@
         <f t="shared" si="0"/>
         <v>0.10503</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="1">
         <f t="shared" si="1"/>
         <v>0.88238259262370833</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
         <v>45744</v>
       </c>
       <c r="B18" t="s">
@@ -932,13 +954,13 @@
         <f t="shared" ref="H18:H32" si="2">D18-G18</f>
         <v>4.8230000000000002E-2</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="1">
         <f t="shared" ref="I18:I32" si="3">H18/D18</f>
         <v>0.88560411311053988</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
         <v>45744</v>
       </c>
       <c r="B19" t="s">
@@ -957,13 +979,13 @@
         <f t="shared" si="2"/>
         <v>5.7249999999999995E-2</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="1">
         <f t="shared" si="3"/>
         <v>0.87618610345883075</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>45744</v>
       </c>
       <c r="B20" t="s">
@@ -982,13 +1004,13 @@
         <f t="shared" si="2"/>
         <v>5.7660000000000003E-2</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="1">
         <f t="shared" si="3"/>
         <v>0.8274971297359357</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>45744</v>
       </c>
       <c r="B21" t="s">
@@ -1007,13 +1029,13 @@
         <f t="shared" si="2"/>
         <v>5.484E-2</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="1">
         <f t="shared" si="3"/>
         <v>0.85155279503105596</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
         <v>45744</v>
       </c>
       <c r="B22" t="s">
@@ -1032,13 +1054,13 @@
         <f t="shared" si="2"/>
         <v>7.5209999999999999E-2</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="1">
         <f t="shared" si="3"/>
         <v>0.90061070530475396</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
         <v>45744</v>
       </c>
       <c r="B23" t="s">
@@ -1057,13 +1079,13 @@
         <f t="shared" si="2"/>
         <v>6.8719999999999989E-2</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="1">
         <f t="shared" si="3"/>
         <v>0.87843538284545564</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
         <v>45744</v>
       </c>
       <c r="B24" t="s">
@@ -1082,13 +1104,13 @@
         <f t="shared" si="2"/>
         <v>0.11238999999999999</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="1">
         <f t="shared" si="3"/>
         <v>0.89876049580167927</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
         <v>45744</v>
       </c>
       <c r="B25" t="s">
@@ -1107,13 +1129,13 @@
         <f t="shared" si="2"/>
         <v>0.10102999999999999</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="1">
         <f t="shared" si="3"/>
         <v>0.94517728505940679</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
         <v>45744</v>
       </c>
       <c r="B26" t="s">
@@ -1132,13 +1154,13 @@
         <f t="shared" si="2"/>
         <v>0.13103999999999999</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="1">
         <f t="shared" si="3"/>
         <v>0.90678845754619053</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
         <v>45744</v>
       </c>
       <c r="B27" t="s">
@@ -1157,13 +1179,13 @@
         <f t="shared" si="2"/>
         <v>7.2160000000000002E-2</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="1">
         <f t="shared" si="3"/>
         <v>0.8796781665244422</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
         <v>45744</v>
       </c>
       <c r="B28" t="s">
@@ -1182,13 +1204,13 @@
         <f t="shared" si="2"/>
         <v>6.6879999999999995E-2</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="1">
         <f t="shared" si="3"/>
         <v>0.89387864207431167</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
         <v>45744</v>
       </c>
       <c r="B29" t="s">
@@ -1207,13 +1229,13 @@
         <f t="shared" si="2"/>
         <v>7.5539999999999996E-2</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="1">
         <f t="shared" si="3"/>
         <v>0.89800285306704708</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
         <v>45744</v>
       </c>
       <c r="B30" t="s">
@@ -1232,13 +1254,13 @@
         <f t="shared" si="2"/>
         <v>2.8580000000000001E-2</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="1">
         <f t="shared" si="3"/>
         <v>0.90443037974683538</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
         <v>45744</v>
       </c>
       <c r="B31" t="s">
@@ -1257,13 +1279,13 @@
         <f t="shared" si="2"/>
         <v>3.3849999999999998E-2</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="1">
         <f t="shared" si="3"/>
         <v>0.88381201044386415</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="1">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
         <v>45744</v>
       </c>
       <c r="B32" t="s">
@@ -1282,13 +1304,13 @@
         <f t="shared" si="2"/>
         <v>4.9570000000000003E-2</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="1">
         <f t="shared" si="3"/>
         <v>0.84547160156916257</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
         <v>45744</v>
       </c>
       <c r="B33" t="s">
@@ -1307,13 +1329,13 @@
         <f t="shared" ref="H33:H62" si="4">D33-G33</f>
         <v>6.5279999999999991E-2</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="1">
         <f t="shared" ref="I33:I62" si="5">H33/D33</f>
         <v>0.87494973864093273</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
         <v>45744</v>
       </c>
       <c r="B34" t="s">
@@ -1332,13 +1354,13 @@
         <f t="shared" si="4"/>
         <v>3.2230000000000002E-2</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34" s="1">
         <f t="shared" si="5"/>
         <v>0.87462686567164183</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="1">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
         <v>45744</v>
       </c>
       <c r="B35" t="s">
@@ -1357,13 +1379,13 @@
         <f t="shared" si="4"/>
         <v>9.426000000000001E-2</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I35" s="1">
         <f t="shared" si="5"/>
         <v>0.88823972860912181</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="1">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
         <v>45744</v>
       </c>
       <c r="B36" t="s">
@@ -1382,13 +1404,13 @@
         <f t="shared" si="4"/>
         <v>6.3390000000000002E-2</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I36" s="1">
         <f t="shared" si="5"/>
         <v>0.90492505353319064</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="1">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
         <v>45744</v>
       </c>
       <c r="B37" t="s">
@@ -1407,13 +1429,13 @@
         <f t="shared" si="4"/>
         <v>5.4610000000000006E-2</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="1">
         <f t="shared" si="5"/>
         <v>0.87348048624440178</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="1">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
         <v>45744</v>
       </c>
       <c r="B38" t="s">
@@ -1432,13 +1454,13 @@
         <f t="shared" si="4"/>
         <v>5.2470000000000003E-2</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I38" s="1">
         <f t="shared" si="5"/>
         <v>0.88022143935581276</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="1">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
         <v>45744</v>
       </c>
       <c r="B39" t="s">
@@ -1457,13 +1479,13 @@
         <f t="shared" si="4"/>
         <v>5.636E-2</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39" s="1">
         <f t="shared" si="5"/>
         <v>0.89602543720190786</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="1">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
         <v>45744</v>
       </c>
       <c r="B40" t="s">
@@ -1482,13 +1504,13 @@
         <f t="shared" si="4"/>
         <v>4.4609999999999997E-2</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I40" s="1">
         <f t="shared" si="5"/>
         <v>0.87694122272459207</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="1">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
         <v>45744</v>
       </c>
       <c r="B41" t="s">
@@ -1507,13 +1529,13 @@
         <f t="shared" si="4"/>
         <v>6.5099999999999991E-2</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41" s="1">
         <f t="shared" si="5"/>
         <v>0.87806851901807381</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="1">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
         <v>45744</v>
       </c>
       <c r="B42" t="s">
@@ -1532,13 +1554,13 @@
         <f t="shared" si="4"/>
         <v>3.7700000000000004E-2</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="1">
         <f t="shared" si="5"/>
         <v>0.85216998191681748</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="1">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
         <v>45744</v>
       </c>
       <c r="B43" t="s">
@@ -1557,13 +1579,13 @@
         <f t="shared" si="4"/>
         <v>0.11572999999999999</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I43" s="1">
         <f t="shared" si="5"/>
         <v>0.88634448954583744</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" s="1">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
         <v>45744</v>
       </c>
       <c r="B44" t="s">
@@ -1582,13 +1604,13 @@
         <f t="shared" si="4"/>
         <v>7.8979999999999995E-2</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I44" s="1">
         <f t="shared" si="5"/>
         <v>0.88117817694968192</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" s="1">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
         <v>45744</v>
       </c>
       <c r="B45" t="s">
@@ -1607,13 +1629,13 @@
         <f t="shared" si="4"/>
         <v>0.10453</v>
       </c>
-      <c r="I45" s="2">
+      <c r="I45" s="1">
         <f t="shared" si="5"/>
         <v>0.88404939106901215</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" s="1">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
         <v>45744</v>
       </c>
       <c r="B46" t="s">
@@ -1632,13 +1654,13 @@
         <f t="shared" si="4"/>
         <v>5.0299999999999997E-2</v>
       </c>
-      <c r="I46" s="2">
+      <c r="I46" s="1">
         <f t="shared" si="5"/>
         <v>0.88183730715287512</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A47" s="1">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
         <v>45744</v>
       </c>
       <c r="B47" t="s">
@@ -1657,13 +1679,13 @@
         <f t="shared" si="4"/>
         <v>9.1730000000000006E-2</v>
       </c>
-      <c r="I47" s="2">
+      <c r="I47" s="1">
         <f t="shared" si="5"/>
         <v>0.87729533282325944</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" s="1">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
         <v>45764</v>
       </c>
       <c r="B48" t="s">
@@ -1682,13 +1704,13 @@
         <f t="shared" si="4"/>
         <v>2.8140000000000002E-2</v>
       </c>
-      <c r="I48" s="2">
+      <c r="I48" s="1">
         <f t="shared" si="5"/>
         <v>0.99294283697953423</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" s="1">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
         <v>45764</v>
       </c>
       <c r="B49" t="s">
@@ -1707,13 +1729,13 @@
         <f t="shared" si="4"/>
         <v>2.8080000000000001E-2</v>
       </c>
-      <c r="I49" s="2">
+      <c r="I49" s="1">
         <f t="shared" si="5"/>
         <v>0.86161399202209266</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" s="1">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
         <v>45764</v>
       </c>
       <c r="B50" t="s">
@@ -1732,13 +1754,13 @@
         <f t="shared" si="4"/>
         <v>3.458E-2</v>
       </c>
-      <c r="I50" s="2">
+      <c r="I50" s="1">
         <f t="shared" si="5"/>
         <v>0.88372093023255816</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51" s="1">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
         <v>45764</v>
       </c>
       <c r="B51" t="s">
@@ -1757,13 +1779,13 @@
         <f t="shared" si="4"/>
         <v>6.4489999999999992E-2</v>
       </c>
-      <c r="I51" s="2">
+      <c r="I51" s="1">
         <f t="shared" si="5"/>
         <v>0.86937179832839029</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52" s="1">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
         <v>45764</v>
       </c>
       <c r="B52" t="s">
@@ -1782,13 +1804,13 @@
         <f t="shared" si="4"/>
         <v>4.0370000000000003E-2</v>
       </c>
-      <c r="I52" s="2">
+      <c r="I52" s="1">
         <f t="shared" si="5"/>
         <v>0.88395007663674185</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" s="1">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
         <v>45764</v>
       </c>
       <c r="B53" t="s">
@@ -1807,13 +1829,13 @@
         <f t="shared" si="4"/>
         <v>9.5219999999999999E-2</v>
       </c>
-      <c r="I53" s="2">
+      <c r="I53" s="1">
         <f t="shared" si="5"/>
         <v>0.90659811482433594</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" s="1">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
         <v>45764</v>
       </c>
       <c r="B54" t="s">
@@ -1832,13 +1854,13 @@
         <f t="shared" si="4"/>
         <v>6.649999999999999E-2</v>
       </c>
-      <c r="I54" s="2">
+      <c r="I54" s="1">
         <f t="shared" si="5"/>
         <v>0.88915630431875914</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A55" s="1">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
         <v>45764</v>
       </c>
       <c r="B55" t="s">
@@ -1857,13 +1879,13 @@
         <f t="shared" si="4"/>
         <v>6.7169999999999994E-2</v>
       </c>
-      <c r="I55" s="2">
+      <c r="I55" s="1">
         <f t="shared" si="5"/>
         <v>0.90684487646820566</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" s="1">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
         <v>45764</v>
       </c>
       <c r="B56" t="s">
@@ -1882,13 +1904,13 @@
         <f t="shared" si="4"/>
         <v>9.4E-2</v>
       </c>
-      <c r="I56" s="2">
+      <c r="I56" s="1">
         <f t="shared" si="5"/>
         <v>0.88888888888888895</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" s="1">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
         <v>45764</v>
       </c>
       <c r="B57" t="s">
@@ -1907,13 +1929,13 @@
         <f t="shared" si="4"/>
         <v>3.669E-2</v>
       </c>
-      <c r="I57" s="2">
+      <c r="I57" s="1">
         <f t="shared" si="5"/>
         <v>0.86370056497175152</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A58" s="1">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
         <v>45764</v>
       </c>
       <c r="B58" t="s">
@@ -1932,13 +1954,13 @@
         <f t="shared" si="4"/>
         <v>1.975E-2</v>
       </c>
-      <c r="I58" s="2">
+      <c r="I58" s="1">
         <f t="shared" si="5"/>
         <v>0.88883888388838883</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A59" s="1">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
         <v>45764</v>
       </c>
       <c r="B59" t="s">
@@ -1957,13 +1979,13 @@
         <f t="shared" si="4"/>
         <v>5.9240000000000001E-2</v>
       </c>
-      <c r="I59" s="2">
+      <c r="I59" s="1">
         <f t="shared" si="5"/>
         <v>0.85805330243337197</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A60" s="1">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
         <v>45764</v>
       </c>
       <c r="B60" t="s">
@@ -1982,13 +2004,13 @@
         <f t="shared" si="4"/>
         <v>5.2769999999999997E-2</v>
       </c>
-      <c r="I60" s="2">
+      <c r="I60" s="1">
         <f t="shared" si="5"/>
         <v>0.86084828711256112</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A61" s="1">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
         <v>45764</v>
       </c>
       <c r="B61" t="s">
@@ -2007,13 +2029,13 @@
         <f t="shared" si="4"/>
         <v>6.9580000000000003E-2</v>
       </c>
-      <c r="I61" s="2">
+      <c r="I61" s="1">
         <f t="shared" si="5"/>
         <v>0.89538025994080561</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A62" s="1">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
         <v>45764</v>
       </c>
       <c r="B62" t="s">
@@ -2032,7 +2054,7 @@
         <f t="shared" si="4"/>
         <v>4.6970000000000005E-2</v>
       </c>
-      <c r="I62" s="2">
+      <c r="I62" s="1">
         <f t="shared" si="5"/>
         <v>0.88372530573847607</v>
       </c>

</xml_diff>